<commit_message>
new results check project results.xlsx
</commit_message>
<xml_diff>
--- a/project results.xlsx
+++ b/project results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\othman\Desktop\Bitcoin_address_identity_inference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613EEFF3-B935-4598-8EE7-8EE0950441AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A697022E-523B-426D-8B09-38616B6F09EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14415" yWindow="3315" windowWidth="21615" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="1620" windowWidth="21615" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>recall</t>
   </si>
@@ -61,6 +61,48 @@
   </si>
   <si>
     <t>original data, 0,1 split, 100% balanced</t>
+  </si>
+  <si>
+    <t>LGBM-2500-20-37</t>
+  </si>
+  <si>
+    <t>SMOTE+RUS(0.1,0.5), 0.1 split</t>
+  </si>
+  <si>
+    <t>SMOTE+RUS, 0.1 split (testing on original data) (training 62k rows each)</t>
+  </si>
+  <si>
+    <t>SMOTE+RUS, 0.1 split (testing on original data) (training 90k rows each)</t>
+  </si>
+  <si>
+    <t>SMOTE+RUS, 0.1 split (testing on original data) (training 72k rows each)</t>
+  </si>
+  <si>
+    <t>RF-100-5</t>
+  </si>
+  <si>
+    <t>original data; 0.25 split</t>
+  </si>
+  <si>
+    <t>RF-1500-20</t>
+  </si>
+  <si>
+    <t>original data; 0.1 split; 100% balanced</t>
+  </si>
+  <si>
+    <t>original data; 0.25 split; 100% balanced</t>
+  </si>
+  <si>
+    <t>BalancedRF-1500-20</t>
+  </si>
+  <si>
+    <t>original data;0.1 split; 100k sample of class 0</t>
+  </si>
+  <si>
+    <t>original data;0.1 split; 200k sample of class 0</t>
+  </si>
+  <si>
+    <t>original data;0.1 split; 60k sample of class 0</t>
   </si>
 </sst>
 </file>
@@ -392,16 +434,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
@@ -507,6 +549,263 @@
         <v>0.75</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>0.85</v>
+      </c>
+      <c r="D6">
+        <v>0.9</v>
+      </c>
+      <c r="E6">
+        <v>0.88</v>
+      </c>
+      <c r="F6">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>0.63</v>
+      </c>
+      <c r="D7">
+        <v>0.72</v>
+      </c>
+      <c r="E7">
+        <v>0.67</v>
+      </c>
+      <c r="F7">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D8">
+        <v>0.68</v>
+      </c>
+      <c r="E8">
+        <v>0.63</v>
+      </c>
+      <c r="F8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0.62</v>
+      </c>
+      <c r="D9">
+        <v>0.72</v>
+      </c>
+      <c r="E9">
+        <v>0.67</v>
+      </c>
+      <c r="F9">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D14">
+        <v>0.62</v>
+      </c>
+      <c r="E14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>0.78</v>
+      </c>
+      <c r="D15">
+        <v>0.72</v>
+      </c>
+      <c r="E15">
+        <v>0.75</v>
+      </c>
+      <c r="F15">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>0.77</v>
+      </c>
+      <c r="D16">
+        <v>0.72</v>
+      </c>
+      <c r="E16">
+        <v>0.74</v>
+      </c>
+      <c r="F16">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>0.68</v>
+      </c>
+      <c r="D17">
+        <v>0.69</v>
+      </c>
+      <c r="E17">
+        <v>0.68</v>
+      </c>
+      <c r="F17">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>0.66</v>
+      </c>
+      <c r="D18">
+        <v>0.66</v>
+      </c>
+      <c r="E18">
+        <v>0.66</v>
+      </c>
+      <c r="F18">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>0.63</v>
+      </c>
+      <c r="D19">
+        <v>0.63</v>
+      </c>
+      <c r="E19">
+        <v>0.63</v>
+      </c>
+      <c r="F19">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>0.77</v>
+      </c>
+      <c r="D22">
+        <v>0.53</v>
+      </c>
+      <c r="E22">
+        <v>0.63</v>
+      </c>
+      <c r="F22">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>0.77</v>
+      </c>
+      <c r="D23">
+        <v>0.38</v>
+      </c>
+      <c r="E23">
+        <v>0.5</v>
+      </c>
+      <c r="F23">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>0.77</v>
+      </c>
+      <c r="D24">
+        <v>0.64</v>
+      </c>
+      <c r="E24">
+        <v>0.7</v>
+      </c>
+      <c r="F24">
+        <v>0.73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>